<commit_message>
update the email process
</commit_message>
<xml_diff>
--- a/TestingData.xlsx
+++ b/TestingData.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{667E8F23-7292-45FF-BF19-FD3508FCA2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
   <si>
     <t>File No.</t>
   </si>
@@ -171,42 +167,201 @@
     <t>The Planning Permission Application is for the proposed construction of High Rise Group development (HRB) consisting of Block A &amp; Block B, Block A: Extended Double Basement (Mechanized Parking ) + Stilt floor (part)/ Ground floor (part) + 10 Floors with 36.0m height - office and Block B: Ground floor + 2 Floors - Shops with 9.0m height of Commercial Building.</t>
   </si>
   <si>
+    <t>3 dwelling units</t>
+  </si>
+  <si>
     <t>comprised in Survey Nos. 27/3A1B, 27/12C, 27/13B, 27/14A, 28/1, 28/3 &amp; 29 of Adambakkam Village within the limits of Greater Chennai Corporation applied by Thiru.Kishore Gokaldas HUF in SBC No. CMDA/PP/HRB/S/0360/2023 dated 18.05.2023.</t>
+  </si>
+  <si>
+    <t>Velachery</t>
+  </si>
+  <si>
+    <t>Guindy</t>
+  </si>
+  <si>
+    <t>5 dwelling units</t>
+  </si>
+  <si>
+    <t>The Planning Permission Application is for the proposed construction of High Rise Group development (HRB) consisting of Block A &amp; Block B, Block A: Extended Double Basement (Mechanized Parking ) + Stilt floor (part)/ Ground floor (part) + 10 Floors with 36.0m height - office and Block B: Ground floor + 2 Floors - Shops with 9.0m height of hospital Building.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +374,194 @@
         <bgColor rgb="FFFFD700"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -243,30 +584,312 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -315,7 +938,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -348,26 +971,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -400,23 +1006,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -578,44 +1167,39 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659DD0ED-0742-4251-BB6C-21E635377ABC}">
-  <dimension ref="A1:T3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="11" width="33.140625" customWidth="1"/>
-    <col min="12" max="12" width="242.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" customWidth="1"/>
-    <col min="15" max="16" width="28.140625" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="20" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.2833333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="16.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="17.425" customWidth="1"/>
+    <col min="6" max="6" width="12.8583333333333" customWidth="1"/>
+    <col min="7" max="7" width="23.1416666666667" customWidth="1"/>
+    <col min="8" max="11" width="33.1416666666667" customWidth="1"/>
+    <col min="12" max="12" width="242.858333333333" customWidth="1"/>
+    <col min="13" max="13" width="18.8583333333333" customWidth="1"/>
+    <col min="14" max="14" width="23.425" customWidth="1"/>
+    <col min="15" max="16" width="28.1416666666667" customWidth="1"/>
+    <col min="17" max="17" width="17.425" customWidth="1"/>
+    <col min="18" max="18" width="15.1416666666667" customWidth="1"/>
+    <col min="19" max="19" width="17.425" customWidth="1"/>
+    <col min="20" max="20" width="20.5666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" ht="15" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,7 +1261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" ht="15" spans="1:20">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -729,17 +1313,17 @@
       <c r="Q2" s="2">
         <v>7373083060</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" ht="15" spans="1:20">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -749,7 +1333,7 @@
       <c r="C3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>45997</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -770,12 +1354,14 @@
       <c r="J3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="L3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>32</v>
@@ -789,25 +1375,217 @@
       <c r="Q3" s="2">
         <v>7373083060</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="15" spans="1:20">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45997</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2">
+        <v>9677133177</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>7373083060</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" ht="15" spans="1:20">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45997</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9677133177</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>7373083060</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:20">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45997</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="2">
+        <v>9677133177</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>7373083060</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" xr:uid="{BFA51816-62A4-4092-8261-7BDE35E75FD1}"/>
-    <hyperlink ref="S2" r:id="rId2" xr:uid="{0BD118C2-DAF2-442E-A9BC-91B0739CCCE4}"/>
-    <hyperlink ref="T2" r:id="rId3" xr:uid="{199756B2-DC34-4A8B-853E-E61BB4496696}"/>
-    <hyperlink ref="R3" r:id="rId4" xr:uid="{AFB954D0-1A0D-4FBB-B1EE-C4FB566263A4}"/>
-    <hyperlink ref="S3" r:id="rId5" xr:uid="{BA7965CC-3808-44B1-B35E-2A1CB9DC4A38}"/>
-    <hyperlink ref="T3" r:id="rId6" xr:uid="{4533350F-3E1D-45D3-BA56-04A634144D75}"/>
+    <hyperlink ref="R2" r:id="rId1" display="View PDF"/>
+    <hyperlink ref="S2" r:id="rId2" display="View Approved Plan"/>
+    <hyperlink ref="T2" r:id="rId3" display="View Approval Letter"/>
+    <hyperlink ref="R3" r:id="rId4" display="View PDF"/>
+    <hyperlink ref="S3" r:id="rId5" display="View Approved Plan"/>
+    <hyperlink ref="T3" r:id="rId6" display="View Approval Letter"/>
+    <hyperlink ref="R4" r:id="rId4" display="View PDF"/>
+    <hyperlink ref="S4" r:id="rId5" display="View Approved Plan"/>
+    <hyperlink ref="T4" r:id="rId6" display="View Approval Letter"/>
+    <hyperlink ref="R5" r:id="rId4" display="View PDF"/>
+    <hyperlink ref="S5" r:id="rId5" display="View Approved Plan"/>
+    <hyperlink ref="T5" r:id="rId6" display="View Approval Letter"/>
+    <hyperlink ref="R6" r:id="rId4" display="View PDF"/>
+    <hyperlink ref="S6" r:id="rId5" display="View Approved Plan"/>
+    <hyperlink ref="T6" r:id="rId6" display="View Approval Letter"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>